<commit_message>
Changed structure - the datalock part now emits earnings, and paymentsdue works out what to pay.
</commit_message>
<xml_diff>
--- a/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/LearnerWithMultipleWithdrawnCommitmentAndOneActiveCommitment.xlsx
+++ b/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/LearnerWithMultipleWithdrawnCommitmentAndOneActiveCommitment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-providerpayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SFA\DasProviderPayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{84B2E200-DB40-4CE1-B2D2-282B4E5EA661}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{84682A10-7497-43A1-B1B4-02FC544D2CD6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="RawEarnings" sheetId="2" r:id="rId2"/>
     <sheet name="RawEarningsMathsAndEnglish" sheetId="3" r:id="rId3"/>
     <sheet name="Datalocks" sheetId="4" r:id="rId4"/>
-    <sheet name="Commitments" sheetId="5" r:id="rId5"/>
+    <sheet name="DatalockValidationErrors" sheetId="6" r:id="rId5"/>
+    <sheet name="Commitments" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="74">
   <si>
     <t>CommitmentId</t>
   </si>
@@ -248,6 +249,9 @@
   </si>
   <si>
     <t>2050503-002</t>
+  </si>
+  <si>
+    <t>RuleId</t>
   </si>
 </sst>
 </file>
@@ -5921,10 +5925,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B586D84F-67B6-426E-A6FD-3F22904F0013}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAC57EC-71F8-44A3-A54A-6DD5C7C43883}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:P9"/>
     </sheetView>
   </sheetViews>

</xml_diff>